<commit_message>
add variety of format
</commit_message>
<xml_diff>
--- a/docs/collections/chokumei/metadata/data.xlsx
+++ b/docs/collections/chokumei/metadata/data.xlsx
@@ -119,7 +119,52 @@
 (大学院経済学研究科助手  小 島 浩 之)</t>
   </si>
   <si>
-    <t>ソート用</t>
+    <t>年</t>
+  </si>
+  <si>
+    <t>アイテムURL</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/document/43f80fa0-cc5d-45fe-9dee-152196995b92</t>
+  </si>
+  <si>
+    <t>viewingDirection</t>
+  </si>
+  <si>
+    <t>http://iiif.io/api/presentation/2#rightToLeftDirection</t>
+  </si>
+  <si>
+    <t>43f80fa0-cc5d-45fe-9dee-152196995b92</t>
+  </si>
+  <si>
+    <t>ソート用項目</t>
+  </si>
+  <si>
+    <t>機械可読ドキュメント</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/api/items/459</t>
+  </si>
+  <si>
+    <t>ウェブサイトURL</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/</t>
+  </si>
+  <si>
+    <t>IIIFマニフェストURI</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif/7/manifest</t>
+  </si>
+  <si>
+    <t>帰属</t>
+  </si>
+  <si>
+    <t>東京大学総合図書館 General Library in the University of Tokyo, JAPAN</t>
+  </si>
+  <si>
+    <t>コレクション</t>
   </si>
   <si>
     <t>サムネイル</t>
@@ -128,55 +173,10 @@
     <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif-img/16/full/200,151/0/default.jpg</t>
   </si>
   <si>
-    <t>マニフェストURI</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif/7/manifest</t>
-  </si>
-  <si>
-    <t>コレクション名</t>
-  </si>
-  <si>
-    <t>43f80fa0-cc5d-45fe-9dee-152196995b92</t>
-  </si>
-  <si>
-    <t>アイテムURL</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/document/43f80fa0-cc5d-45fe-9dee-152196995b92</t>
-  </si>
-  <si>
-    <t>サイトURL</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/</t>
-  </si>
-  <si>
-    <t>機械可読データ</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/api/items/459</t>
-  </si>
-  <si>
     <t>利用条件</t>
   </si>
   <si>
     <t>https://www.lib.u-tokyo.ac.jp/ja/library/general/reuse</t>
-  </si>
-  <si>
-    <t>所蔵</t>
-  </si>
-  <si>
-    <t>東京大学総合図書館 General Library in the University of Tokyo, JAPAN</t>
-  </si>
-  <si>
-    <t>viewingDirection</t>
-  </si>
-  <si>
-    <t>http://iiif.io/api/presentation/2#rightToLeftDirection</t>
-  </si>
-  <si>
-    <t>年</t>
   </si>
   <si>
     <t>sc:viewingHint</t>
@@ -594,10 +594,10 @@
         <v>30</v>
       </c>
       <c r="R1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="S1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="T1" t="s">
         <v>34</v>
@@ -615,10 +615,10 @@
         <v>42</v>
       </c>
       <c r="Y1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA1" t="s">
         <v>47</v>
@@ -677,10 +677,7 @@
         <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>35</v>
@@ -691,14 +688,17 @@
       <c r="V2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" t="s">
         <v>41</v>
       </c>
       <c r="X2" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>48</v>
@@ -713,12 +713,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="Q2" r:id="rId2"/>
+    <hyperlink ref="Q2" r:id="rId2" location="rightToLeftDirection"/>
     <hyperlink ref="T2" r:id="rId3"/>
     <hyperlink ref="U2" r:id="rId4"/>
     <hyperlink ref="V2" r:id="rId5"/>
-    <hyperlink ref="W2" r:id="rId6"/>
-    <hyperlink ref="Y2" r:id="rId7" location="rightToLeftDirection"/>
+    <hyperlink ref="Y2" r:id="rId6"/>
+    <hyperlink ref="Z2" r:id="rId7"/>
     <hyperlink ref="AA2" r:id="rId8" location="nonPagedHint"/>
     <hyperlink ref="AB2" r:id="rId9"/>
     <hyperlink ref="AC2" r:id="rId10"/>

</xml_diff>

<commit_message>
update logic to create data
</commit_message>
<xml_diff>
--- a/docs/collections/chokumei/metadata/data.xlsx
+++ b/docs/collections/chokumei/metadata/data.xlsx
@@ -14,60 +14,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>タイトル</t>
   </si>
   <si>
+    <t>dcterms:title</t>
+  </si>
+  <si>
     <t>明・弘治十八年八月二十日勅命</t>
   </si>
   <si>
     <t>請求記号</t>
   </si>
   <si>
+    <t>dcndl:callNumber</t>
+  </si>
+  <si>
     <t>鴎A00:6270</t>
   </si>
   <si>
     <t>登録番号</t>
   </si>
   <si>
+    <t>dcndl:sourceIdentifier</t>
+  </si>
+  <si>
     <t>0004804951</t>
   </si>
   <si>
     <t>状態</t>
   </si>
   <si>
+    <t>dcterms:type</t>
+  </si>
+  <si>
     <t>貴重本</t>
   </si>
   <si>
-    <t>uterms:bunko</t>
-  </si>
-  <si>
-    <t>鴎外文庫</t>
-  </si>
-  <si>
     <t>出版者</t>
   </si>
   <si>
+    <t>dcterms:publisher</t>
+  </si>
+  <si>
     <t>[製作地不明] : [製作者不明]</t>
   </si>
   <si>
     <t>出版年</t>
   </si>
   <si>
+    <t>dcterms:date</t>
+  </si>
+  <si>
     <t>弘治18 [1505]</t>
   </si>
   <si>
     <t>大きさ</t>
   </si>
   <si>
+    <t>dcterms:extent</t>
+  </si>
+  <si>
     <t>1軸 ; 33cm</t>
   </si>
   <si>
     <t>別書名</t>
   </si>
   <si>
+    <t>dcndl:alternative</t>
+  </si>
+  <si>
     <t>一般注記</t>
+  </si>
+  <si>
+    <t>archiveshub:note</t>
   </si>
   <si>
     <t>和漢古書につき記述対象資料毎に書誌レコード作成_x000D_
@@ -83,22 +104,34 @@
     <t>著者標目</t>
   </si>
   <si>
+    <t>dcterms:creator</t>
+  </si>
+  <si>
     <t>孝宗 &lt;コウソウ&gt; &lt;xiao zong&gt;</t>
   </si>
   <si>
     <t>本文言語</t>
   </si>
   <si>
+    <t>dcterms:language</t>
+  </si>
+  <si>
     <t>中国語</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>dcterms:identifier</t>
+  </si>
+  <si>
     <t>2002618266|BA87193508</t>
   </si>
   <si>
     <t>解説</t>
+  </si>
+  <si>
+    <t>dcterms:description</t>
   </si>
   <si>
     <t>解題 明・弘治十八年八月二十日勅命(東京大学東京大学総合図書館所蔵鴎外文庫本)_x000D_
@@ -119,82 +152,139 @@
 (大学院経済学研究科助手  小 島 浩 之)</t>
   </si>
   <si>
-    <t>年</t>
+    <t>文庫区分</t>
+  </si>
+  <si>
+    <t>uterms:bunko</t>
+  </si>
+  <si>
+    <t>鴎外文庫</t>
+  </si>
+  <si>
+    <t>viewingHint</t>
+  </si>
+  <si>
+    <t>sc:viewingHint</t>
+  </si>
+  <si>
+    <t>http://iiif.io/api/presentation/2#nonPagedHint</t>
+  </si>
+  <si>
+    <t>Annotated Manifest</t>
+  </si>
+  <si>
+    <t>uterms:annotedManifest</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/omekac/oa/collections/1/manifest.json</t>
+  </si>
+  <si>
+    <t>Search Api Uri</t>
+  </si>
+  <si>
+    <t>uterms:searchApiUri</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/api/iiif-search/kPzFpI4mtex7HdRmrZL1ew9r7OCgdDPvNX2g0njpVtAboi6IrB%EF%BC%8FuxrlG%EF%BC%8FWAUZQNUKk%EF%BC%8BfS5OHRkhqjeP9kEbj%EF%BC%8FdLhnZBYlvz3IMieAyKPg20%3D</t>
+  </si>
+  <si>
+    <t>bibo:identifier</t>
+  </si>
+  <si>
+    <t>43f80fa0-cc5d-45fe-9dee-152196995b92</t>
+  </si>
+  <si>
+    <t>ウェブサイトURL</t>
+  </si>
+  <si>
+    <t>dcterms:isPartOf</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/</t>
   </si>
   <si>
     <t>アイテムURL</t>
   </si>
   <si>
+    <t>dcterms:relation</t>
+  </si>
+  <si>
     <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/document/43f80fa0-cc5d-45fe-9dee-152196995b92</t>
   </si>
   <si>
+    <t>利用条件</t>
+  </si>
+  <si>
+    <t>dcterms:rights</t>
+  </si>
+  <si>
+    <t>https://www.lib.u-tokyo.ac.jp/ja/library/general/reuse</t>
+  </si>
+  <si>
+    <t>サムネイル</t>
+  </si>
+  <si>
+    <t>foaf:thumbnail</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif-img/16/full/200,151/0/default.jpg</t>
+  </si>
+  <si>
+    <t>機械可読ドキュメント</t>
+  </si>
+  <si>
+    <t>rdfs:seeAlso</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/api/items/459</t>
+  </si>
+  <si>
+    <t>帰属</t>
+  </si>
+  <si>
+    <t>sc:attributionLabel</t>
+  </si>
+  <si>
+    <t>東京大学総合図書館 General Library in the University of Tokyo, JAPAN</t>
+  </si>
+  <si>
     <t>viewingDirection</t>
   </si>
   <si>
+    <t>sc:viewingDirection</t>
+  </si>
+  <si>
     <t>http://iiif.io/api/presentation/2#rightToLeftDirection</t>
   </si>
   <si>
-    <t>43f80fa0-cc5d-45fe-9dee-152196995b92</t>
+    <t>コレクション</t>
+  </si>
+  <si>
+    <t>uterms:databaseLabel</t>
+  </si>
+  <si>
+    <t>IIIFマニフェストURI</t>
+  </si>
+  <si>
+    <t>uterms:manifestUri</t>
+  </si>
+  <si>
+    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif/43f80fa0-cc5d-45fe-9dee-152196995b92/manifest</t>
   </si>
   <si>
     <t>ソート用項目</t>
   </si>
   <si>
-    <t>機械可読ドキュメント</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/api/items/459</t>
-  </si>
-  <si>
-    <t>ウェブサイトURL</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/s/chokumei/</t>
-  </si>
-  <si>
-    <t>IIIFマニフェストURI</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif/7/manifest</t>
-  </si>
-  <si>
-    <t>帰属</t>
-  </si>
-  <si>
-    <t>東京大学総合図書館 General Library in the University of Tokyo, JAPAN</t>
-  </si>
-  <si>
-    <t>コレクション</t>
-  </si>
-  <si>
-    <t>サムネイル</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/repo/iiif-img/16/full/200,151/0/default.jpg</t>
-  </si>
-  <si>
-    <t>利用条件</t>
-  </si>
-  <si>
-    <t>https://www.lib.u-tokyo.ac.jp/ja/library/general/reuse</t>
-  </si>
-  <si>
-    <t>sc:viewingHint</t>
-  </si>
-  <si>
-    <t>http://iiif.io/api/presentation/2#nonPagedHint</t>
-  </si>
-  <si>
-    <t>uterms:annotedManifest</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/omekac/oa/collections/1/manifest.json</t>
-  </si>
-  <si>
-    <t>uterms:searchApiUri</t>
-  </si>
-  <si>
-    <t>https://iiif.dl.itc.u-tokyo.ac.jp/api/iiif-search/kPzFpI4mtex7HdRmrZL1ew9r7OCgdDPvNX2g0njpVtAboi6IrB%EF%BC%8FuxrlG%EF%BC%8FWAUZQNUKk%EF%BC%8BfS5OHRkhqjeP9kEbj%EF%BC%8FdLhnZBYlvz3IMieAyKPg20%3D</t>
+    <t>uterms:sort</t>
+  </si>
+  <si>
+    <t>西暦</t>
+  </si>
+  <si>
+    <t>uterms:year</t>
+  </si>
+  <si>
+    <t># of media</t>
   </si>
 </sst>
 </file>
@@ -212,10 +302,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -235,14 +324,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,193 +629,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="M1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="R1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="T1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="U1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="V1" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="W1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="X1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="Y1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="Z1" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="AA1" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="AB1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="AC1" t="s">
-        <v>51</v>
+        <v>80</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" s="1" t="s">
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>52</v>
+      <c r="Q3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="Q2" r:id="rId2" location="rightToLeftDirection"/>
-    <hyperlink ref="T2" r:id="rId3"/>
-    <hyperlink ref="U2" r:id="rId4"/>
-    <hyperlink ref="V2" r:id="rId5"/>
-    <hyperlink ref="Y2" r:id="rId6"/>
-    <hyperlink ref="Z2" r:id="rId7"/>
-    <hyperlink ref="AA2" r:id="rId8" location="nonPagedHint"/>
-    <hyperlink ref="AB2" r:id="rId9"/>
-    <hyperlink ref="AC2" r:id="rId10"/>
+    <hyperlink ref="O3" r:id="rId1" location="nonPagedHint"/>
+    <hyperlink ref="P3" r:id="rId2"/>
+    <hyperlink ref="Q3" r:id="rId3"/>
+    <hyperlink ref="S3" r:id="rId4"/>
+    <hyperlink ref="T3" r:id="rId5"/>
+    <hyperlink ref="U3" r:id="rId6"/>
+    <hyperlink ref="V3" r:id="rId7"/>
+    <hyperlink ref="W3" r:id="rId8"/>
+    <hyperlink ref="Y3" r:id="rId9" location="rightToLeftDirection"/>
+    <hyperlink ref="AA3" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>